<commit_message>
Fixed and updated the OneStopShop
</commit_message>
<xml_diff>
--- a/TestBook.xlsx
+++ b/TestBook.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="2780" yWindow="1560"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17440" windowWidth="28040" xWindow="2780" yWindow="1560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="taken" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="taken1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="aggregate_data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="aggregate_data1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -364,8 +365,8 @@
   </sheetPr>
   <dimension ref="A1:BY18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2669,7 +2670,7 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2691,7 +2692,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -2832,6 +2833,147 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>donor_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>committee_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>aggregate_amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ADAMS, DANY</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PROGRESSIVE TURNOUT PROJECT</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ADAMS, DANY</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ACTBLUE</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GRAHAM, JULIE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PROGRESSIVE TURNOUT PROJECT</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OLUM, KEN</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ELIZABETH PANNILL FLETCHER FOR CONGRESS</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BACHOVCHIN, WILLIAM</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TRUMP MAKE AMERICA GREAT AGAIN COMMITTEE</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>KATES-GARNICK, BARBARA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TINA SMITH FOR MINNESOTA</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AIKENS, KRISTINA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ACTBLUE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">

</xml_diff>